<commit_message>
Added missing email address to class list
</commit_message>
<xml_diff>
--- a/classlist.xlsx
+++ b/classlist.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="322">
   <si>
     <t>SPRING TERM 2015-2016      Registration Class List     03-FEB-16       6.S062   U</t>
   </si>
@@ -982,6 +982,9 @@
   </si>
   <si>
     <t>dumesnil@mit.edu</t>
+  </si>
+  <si>
+    <t>lucasms@mit.edu</t>
   </si>
 </sst>
 </file>
@@ -1462,7 +1465,7 @@
   <dimension ref="A1:AM37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+      <selection activeCell="AJ30" sqref="AJ30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3112,6 +3115,9 @@
       <c r="D30" s="1">
         <v>4</v>
       </c>
+      <c r="J30" t="s">
+        <v>321</v>
+      </c>
       <c r="AJ30" t="s">
         <v>291</v>
       </c>

</xml_diff>

<commit_message>
More class list updates
</commit_message>
<xml_diff>
--- a/classlist.xlsx
+++ b/classlist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28780" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="classlst.xls" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="321">
   <si>
     <t>SPRING TERM 2015-2016      Registration Class List     03-FEB-16       6.S062   U</t>
   </si>
@@ -135,51 +135,9 @@
     <t>Confid</t>
   </si>
   <si>
-    <t>_______</t>
-  </si>
-  <si>
-    <t>____________</t>
-  </si>
-  <si>
-    <t>____</t>
-  </si>
-  <si>
-    <t>______</t>
-  </si>
-  <si>
-    <t>_____</t>
-  </si>
-  <si>
-    <t>________</t>
-  </si>
-  <si>
-    <t>_____________</t>
-  </si>
-  <si>
-    <t>________________</t>
-  </si>
-  <si>
-    <t>_________________</t>
-  </si>
-  <si>
-    <t>__________</t>
-  </si>
-  <si>
-    <t>_________</t>
-  </si>
-  <si>
-    <t>___________</t>
-  </si>
-  <si>
-    <t>__________________</t>
-  </si>
-  <si>
     <t xml:space="preserve">Blalock,Davis </t>
   </si>
   <si>
-    <t xml:space="preserve">   6 D</t>
-  </si>
-  <si>
     <t>G</t>
   </si>
   <si>
@@ -189,9 +147,6 @@
     <t>LIS</t>
   </si>
   <si>
-    <t xml:space="preserve">  6.S062</t>
-  </si>
-  <si>
     <t>dblalock@MIT.EDU</t>
   </si>
   <si>
@@ -228,9 +183,6 @@
     <t>Brettin,Jorrie M.</t>
   </si>
   <si>
-    <t xml:space="preserve">   6 3</t>
-  </si>
-  <si>
     <t>Reg</t>
   </si>
   <si>
@@ -267,9 +219,6 @@
     <t>Chang,Brendan S.</t>
   </si>
   <si>
-    <t xml:space="preserve">   6 2</t>
-  </si>
-  <si>
     <t>bschang@MIT.EDU</t>
   </si>
   <si>
@@ -444,9 +393,6 @@
     <t>Gupta,Ankush M.</t>
   </si>
   <si>
-    <t xml:space="preserve">   6 P</t>
-  </si>
-  <si>
     <t>ankush@MIT.EDU</t>
   </si>
   <si>
@@ -474,9 +420,6 @@
     <t>Helbert,Kendall L.</t>
   </si>
   <si>
-    <t xml:space="preserve">   2 A</t>
-  </si>
-  <si>
     <t>khelbert@MIT.EDU</t>
   </si>
   <si>
@@ -951,9 +894,6 @@
     <t>Staff</t>
   </si>
   <si>
-    <t>Bartel,Katie</t>
-  </si>
-  <si>
     <t>Kini,Keertan</t>
   </si>
   <si>
@@ -991,6 +931,57 @@
   </si>
   <si>
     <t>Withdrew 2/6/16</t>
+  </si>
+  <si>
+    <t>Bartel,Kathryn W.</t>
+  </si>
+  <si>
+    <t>6.S062</t>
+  </si>
+  <si>
+    <t>Freel,Austin E.</t>
+  </si>
+  <si>
+    <t>afreel@MIT.EDU</t>
+  </si>
+  <si>
+    <t>Can</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>Nordin,Alexander F</t>
+  </si>
+  <si>
+    <t>anordin@MIT.EDU</t>
+  </si>
+  <si>
+    <t>Subramanyam,Hariha</t>
+  </si>
+  <si>
+    <t>hsubrama@MIT.EDU</t>
+  </si>
+  <si>
+    <t>6 2</t>
+  </si>
+  <si>
+    <t>6 D</t>
+  </si>
+  <si>
+    <t>6 3</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>6 P</t>
+  </si>
+  <si>
+    <t>2 A</t>
+  </si>
+  <si>
+    <t>Cancelled by 2/7/16</t>
   </si>
 </sst>
 </file>
@@ -1049,7 +1040,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1057,8 +1048,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="39">
+  <cellStyleXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1098,8 +1098,72 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1110,8 +1174,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="39">
+  <cellStyles count="103">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1132,6 +1200,38 @@
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1150,6 +1250,38 @@
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1479,21 +1611,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AN37"/>
+  <dimension ref="A1:AN39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AK27" sqref="AK27"/>
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.1640625" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" style="6" customWidth="1"/>
     <col min="4" max="4" width="7.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="6.1640625" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="9.1640625" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="8.1640625" hidden="1" customWidth="1"/>
+    <col min="6" max="7" width="6.1640625" customWidth="1"/>
+    <col min="8" max="8" width="9.1640625" customWidth="1"/>
+    <col min="9" max="9" width="8.1640625" customWidth="1"/>
     <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20" hidden="1" customWidth="1"/>
     <col min="12" max="35" width="10.83203125" hidden="1" customWidth="1"/>
@@ -1517,362 +1649,329 @@
       </c>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:40">
-      <c r="A4" t="s">
+    <row r="4" spans="1:40" s="7" customFormat="1" ht="16" thickBot="1">
+      <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="O4" t="s">
+      <c r="O4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="P4" t="s">
+      <c r="P4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="Q4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="R4" t="s">
+      <c r="R4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="S4" t="s">
+      <c r="S4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="T4" t="s">
+      <c r="T4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="U4" t="s">
+      <c r="U4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="V4" t="s">
+      <c r="V4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="W4" t="s">
+      <c r="W4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="X4" t="s">
+      <c r="X4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="Y4" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="Z4" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AA4" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AB4" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AC4" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AD4" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AE4" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="AF4" t="s">
+      <c r="AF4" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="AG4" t="s">
+      <c r="AG4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="AH4" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="AI4" t="s">
+      <c r="AI4" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="AJ4" t="s">
-        <v>294</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>295</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>296</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>297</v>
-      </c>
-      <c r="AN4" t="s">
-        <v>322</v>
+      <c r="AJ4" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="AK4" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="AL4" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="AM4" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="AN4" s="7" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="5" spans="1:40">
-      <c r="A5" t="s">
-        <v>38</v>
+      <c r="A5">
+        <v>924301388</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" t="s">
-        <v>40</v>
+        <v>304</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="D5" s="1">
+        <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F5" t="s">
-        <v>42</v>
-      </c>
-      <c r="G5" t="s">
-        <v>42</v>
+        <v>54</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>43</v>
-      </c>
-      <c r="I5" t="s">
-        <v>38</v>
-      </c>
-      <c r="J5" t="s">
-        <v>44</v>
-      </c>
-      <c r="K5" t="s">
-        <v>39</v>
-      </c>
-      <c r="L5" t="s">
-        <v>44</v>
-      </c>
-      <c r="M5" t="s">
-        <v>45</v>
-      </c>
-      <c r="N5" t="s">
-        <v>46</v>
-      </c>
-      <c r="O5" t="s">
-        <v>39</v>
-      </c>
-      <c r="P5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>47</v>
-      </c>
-      <c r="R5" t="s">
-        <v>44</v>
-      </c>
-      <c r="S5" t="s">
-        <v>44</v>
-      </c>
-      <c r="T5" t="s">
-        <v>44</v>
-      </c>
-      <c r="U5" t="s">
-        <v>48</v>
-      </c>
-      <c r="V5" t="s">
-        <v>47</v>
-      </c>
-      <c r="W5" t="s">
-        <v>43</v>
-      </c>
-      <c r="X5" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>50</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>44</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>44</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>48</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>47</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>43</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>48</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>49</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>41</v>
+        <v>305</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>297</v>
       </c>
       <c r="AJ5" t="s">
-        <v>42</v>
+        <v>270</v>
       </c>
       <c r="AK5" t="s">
-        <v>42</v>
+        <v>270</v>
       </c>
       <c r="AL5" t="s">
-        <v>42</v>
+        <v>270</v>
       </c>
       <c r="AM5" t="s">
-        <v>39</v>
+        <v>270</v>
       </c>
     </row>
     <row r="6" spans="1:40">
+      <c r="A6">
+        <v>916523598</v>
+      </c>
       <c r="B6" t="s">
-        <v>310</v>
-      </c>
-      <c r="D6" s="1">
-        <v>4</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>317</v>
+        <v>38</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="E6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" t="s">
+        <v>305</v>
+      </c>
+      <c r="J6" t="s">
+        <v>42</v>
+      </c>
+      <c r="K6" t="s">
+        <v>43</v>
+      </c>
+      <c r="L6" t="s">
+        <v>44</v>
+      </c>
+      <c r="O6" t="s">
+        <v>45</v>
+      </c>
+      <c r="P6" t="s">
+        <v>46</v>
+      </c>
+      <c r="R6" t="s">
+        <v>47</v>
+      </c>
+      <c r="U6" t="s">
+        <v>48</v>
+      </c>
+      <c r="V6" t="s">
+        <v>49</v>
+      </c>
+      <c r="W6">
+        <v>2139</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF6">
+        <v>22901</v>
       </c>
       <c r="AJ6" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
       <c r="AK6" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
       <c r="AL6" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
       <c r="AM6" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
     </row>
     <row r="7" spans="1:40">
       <c r="A7">
-        <v>916523598</v>
+        <v>917227233</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>288</v>
+        <v>53</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="D7" s="1">
+        <v>4</v>
       </c>
       <c r="E7" t="s">
         <v>54</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" t="s">
+        <v>305</v>
+      </c>
+      <c r="J7" t="s">
         <v>55</v>
       </c>
-      <c r="H7" t="s">
+      <c r="K7" t="s">
         <v>56</v>
       </c>
-      <c r="J7" t="s">
+      <c r="L7" t="s">
         <v>57</v>
       </c>
-      <c r="K7" t="s">
+      <c r="O7" t="s">
         <v>58</v>
       </c>
-      <c r="L7" t="s">
+      <c r="P7" t="s">
         <v>59</v>
       </c>
-      <c r="O7" t="s">
+      <c r="Q7" t="s">
         <v>60</v>
       </c>
-      <c r="P7" t="s">
+      <c r="AA7" t="s">
         <v>61</v>
       </c>
-      <c r="R7" t="s">
+      <c r="AB7" t="s">
         <v>62</v>
       </c>
-      <c r="U7" t="s">
+      <c r="AD7" t="s">
         <v>63</v>
       </c>
-      <c r="V7" t="s">
+      <c r="AE7" t="s">
         <v>64</v>
       </c>
-      <c r="W7">
-        <v>2139</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>65</v>
-      </c>
-      <c r="AD7" t="s">
-        <v>66</v>
-      </c>
-      <c r="AE7" t="s">
-        <v>67</v>
-      </c>
       <c r="AF7">
-        <v>22901</v>
+        <v>58718</v>
       </c>
       <c r="AJ7" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
       <c r="AK7" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
       <c r="AL7" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
       <c r="AM7" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
     </row>
     <row r="8" spans="1:40">
       <c r="A8">
-        <v>917227233</v>
+        <v>911027923</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
-      </c>
-      <c r="C8" t="s">
-        <v>69</v>
-      </c>
-      <c r="D8" s="1">
-        <v>4</v>
+        <v>65</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>271</v>
       </c>
       <c r="E8" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="F8">
         <v>12</v>
@@ -1881,183 +1980,210 @@
         <v>2</v>
       </c>
       <c r="H8" t="s">
-        <v>56</v>
+        <v>305</v>
       </c>
       <c r="J8" t="s">
+        <v>66</v>
+      </c>
+      <c r="K8" t="s">
+        <v>67</v>
+      </c>
+      <c r="L8" t="s">
+        <v>68</v>
+      </c>
+      <c r="O8" t="s">
+        <v>69</v>
+      </c>
+      <c r="P8" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q8" t="s">
         <v>71</v>
       </c>
-      <c r="K8" t="s">
+      <c r="AA8" t="s">
         <v>72</v>
       </c>
-      <c r="L8" t="s">
+      <c r="AD8" t="s">
         <v>73</v>
       </c>
-      <c r="O8" t="s">
+      <c r="AE8" t="s">
         <v>74</v>
       </c>
-      <c r="P8" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>76</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>77</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>78</v>
-      </c>
-      <c r="AD8" t="s">
-        <v>79</v>
-      </c>
-      <c r="AE8" t="s">
-        <v>80</v>
-      </c>
       <c r="AF8">
-        <v>58718</v>
+        <v>20882</v>
       </c>
       <c r="AJ8" t="s">
-        <v>289</v>
+        <v>272</v>
       </c>
       <c r="AK8" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
       <c r="AL8" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
       <c r="AM8" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
     </row>
     <row r="9" spans="1:40">
-      <c r="A9">
-        <v>911027923</v>
-      </c>
       <c r="B9" t="s">
-        <v>81</v>
-      </c>
-      <c r="C9" t="s">
-        <v>82</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="E9" t="s">
-        <v>70</v>
-      </c>
-      <c r="F9">
-        <v>12</v>
-      </c>
-      <c r="G9" t="s">
-        <v>2</v>
+        <v>284</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="D9" s="1">
+        <v>3</v>
       </c>
       <c r="H9" t="s">
-        <v>56</v>
+        <v>317</v>
       </c>
       <c r="J9" t="s">
-        <v>83</v>
-      </c>
-      <c r="K9" t="s">
-        <v>84</v>
-      </c>
-      <c r="L9" t="s">
-        <v>85</v>
-      </c>
-      <c r="O9" t="s">
-        <v>86</v>
-      </c>
-      <c r="P9" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>88</v>
-      </c>
-      <c r="AA9" t="s">
-        <v>89</v>
-      </c>
-      <c r="AD9" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AF9">
-        <v>20882</v>
+        <v>285</v>
       </c>
       <c r="AJ9" t="s">
-        <v>291</v>
+        <v>273</v>
       </c>
       <c r="AK9" t="s">
-        <v>292</v>
+        <v>270</v>
       </c>
       <c r="AL9" t="s">
-        <v>292</v>
+        <v>270</v>
       </c>
       <c r="AM9" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
     </row>
     <row r="10" spans="1:40">
+      <c r="A10">
+        <v>920359511</v>
+      </c>
       <c r="B10" t="s">
-        <v>303</v>
+        <v>283</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>314</v>
       </c>
       <c r="D10" s="1">
         <v>3</v>
       </c>
+      <c r="E10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10">
+        <v>12</v>
+      </c>
+      <c r="H10" t="s">
+        <v>305</v>
+      </c>
       <c r="J10" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="AJ10" t="s">
-        <v>292</v>
+        <v>272</v>
       </c>
       <c r="AK10" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
       <c r="AL10" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
       <c r="AM10" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
     </row>
     <row r="11" spans="1:40">
+      <c r="A11">
+        <v>921761487</v>
+      </c>
       <c r="B11" t="s">
-        <v>302</v>
+        <v>75</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>314</v>
       </c>
       <c r="D11" s="1">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="E11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11">
+        <v>12</v>
+      </c>
+      <c r="G11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" t="s">
+        <v>305</v>
       </c>
       <c r="J11" t="s">
-        <v>320</v>
+        <v>76</v>
+      </c>
+      <c r="K11" t="s">
+        <v>77</v>
+      </c>
+      <c r="L11" t="s">
+        <v>78</v>
+      </c>
+      <c r="M11" t="s">
+        <v>79</v>
+      </c>
+      <c r="N11" t="s">
+        <v>80</v>
+      </c>
+      <c r="O11" t="s">
+        <v>81</v>
+      </c>
+      <c r="P11" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>83</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>86</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>87</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>88</v>
       </c>
       <c r="AJ11" t="s">
-        <v>291</v>
+        <v>272</v>
       </c>
       <c r="AK11" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
       <c r="AL11" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
       <c r="AM11" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
     </row>
     <row r="12" spans="1:40">
       <c r="A12">
-        <v>921761487</v>
+        <v>919051432</v>
       </c>
       <c r="B12" t="s">
-        <v>92</v>
-      </c>
-      <c r="C12" t="s">
-        <v>82</v>
+        <v>89</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>316</v>
       </c>
       <c r="D12" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E12" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="F12">
         <v>12</v>
@@ -2066,164 +2192,119 @@
         <v>2</v>
       </c>
       <c r="H12" t="s">
-        <v>56</v>
+        <v>305</v>
       </c>
       <c r="J12" t="s">
+        <v>90</v>
+      </c>
+      <c r="K12" t="s">
+        <v>91</v>
+      </c>
+      <c r="L12" t="s">
+        <v>92</v>
+      </c>
+      <c r="O12" t="s">
         <v>93</v>
       </c>
-      <c r="K12" t="s">
+      <c r="P12" t="s">
         <v>94</v>
       </c>
-      <c r="L12" t="s">
+      <c r="Q12" t="s">
         <v>95</v>
       </c>
-      <c r="M12" t="s">
+      <c r="R12" t="s">
         <v>96</v>
       </c>
-      <c r="N12" t="s">
+      <c r="U12" t="s">
         <v>97</v>
       </c>
-      <c r="O12" t="s">
+      <c r="V12" t="s">
+        <v>49</v>
+      </c>
+      <c r="W12">
+        <v>2134</v>
+      </c>
+      <c r="Z12" t="s">
         <v>98</v>
       </c>
-      <c r="P12" t="s">
+      <c r="AA12" t="s">
         <v>99</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="AD12" t="s">
         <v>100</v>
       </c>
-      <c r="AA12" t="s">
+      <c r="AE12" t="s">
         <v>101</v>
       </c>
-      <c r="AB12" t="s">
-        <v>102</v>
-      </c>
-      <c r="AC12" t="s">
-        <v>103</v>
-      </c>
-      <c r="AD12" t="s">
-        <v>104</v>
-      </c>
-      <c r="AH12" t="s">
-        <v>105</v>
+      <c r="AF12">
+        <v>95448</v>
       </c>
       <c r="AJ12" t="s">
-        <v>291</v>
+        <v>274</v>
       </c>
       <c r="AK12" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
       <c r="AL12" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
       <c r="AM12" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
     </row>
     <row r="13" spans="1:40">
-      <c r="A13">
-        <v>919051432</v>
-      </c>
       <c r="B13" t="s">
-        <v>106</v>
-      </c>
-      <c r="C13" t="s">
-        <v>69</v>
-      </c>
-      <c r="D13" s="1">
-        <v>3</v>
-      </c>
-      <c r="E13" t="s">
-        <v>70</v>
-      </c>
-      <c r="F13">
-        <v>12</v>
-      </c>
-      <c r="G13" t="s">
-        <v>2</v>
+        <v>288</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>290</v>
       </c>
       <c r="H13" t="s">
-        <v>56</v>
+        <v>317</v>
       </c>
       <c r="J13" t="s">
-        <v>107</v>
-      </c>
-      <c r="K13" t="s">
-        <v>108</v>
-      </c>
-      <c r="L13" t="s">
-        <v>109</v>
-      </c>
-      <c r="O13" t="s">
-        <v>110</v>
-      </c>
-      <c r="P13" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>112</v>
-      </c>
-      <c r="R13" t="s">
-        <v>113</v>
-      </c>
-      <c r="U13" t="s">
-        <v>114</v>
-      </c>
-      <c r="V13" t="s">
-        <v>64</v>
-      </c>
-      <c r="W13">
-        <v>2134</v>
-      </c>
-      <c r="Z13" t="s">
-        <v>115</v>
-      </c>
-      <c r="AA13" t="s">
-        <v>116</v>
-      </c>
-      <c r="AD13" t="s">
-        <v>117</v>
-      </c>
-      <c r="AE13" t="s">
-        <v>118</v>
-      </c>
-      <c r="AF13">
-        <v>95448</v>
+        <v>289</v>
       </c>
       <c r="AJ13" t="s">
-        <v>293</v>
+        <v>273</v>
       </c>
       <c r="AK13" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
       <c r="AL13" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
       <c r="AM13" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
     </row>
     <row r="14" spans="1:40">
+      <c r="A14">
+        <v>926490698</v>
+      </c>
       <c r="B14" t="s">
+        <v>306</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14">
+        <v>12</v>
+      </c>
+      <c r="H14" t="s">
+        <v>305</v>
+      </c>
+      <c r="J14" t="s">
         <v>307</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="J14" t="s">
-        <v>308</v>
-      </c>
-      <c r="AJ14" t="s">
-        <v>292</v>
-      </c>
-      <c r="AK14" t="s">
-        <v>289</v>
-      </c>
-      <c r="AL14" t="s">
-        <v>292</v>
-      </c>
-      <c r="AM14" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="15" spans="1:40">
@@ -2231,16 +2312,16 @@
         <v>927850236</v>
       </c>
       <c r="B15" t="s">
-        <v>119</v>
-      </c>
-      <c r="C15" t="s">
-        <v>82</v>
+        <v>102</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>314</v>
       </c>
       <c r="D15" s="1">
         <v>4</v>
       </c>
       <c r="E15" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="F15">
         <v>12</v>
@@ -2249,52 +2330,52 @@
         <v>2</v>
       </c>
       <c r="H15" t="s">
-        <v>56</v>
+        <v>305</v>
       </c>
       <c r="J15" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="K15" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="L15" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="M15" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="N15" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="O15" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="P15" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="AA15" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="AB15" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="AD15" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="AH15" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="AJ15" t="s">
-        <v>291</v>
+        <v>272</v>
       </c>
       <c r="AK15" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
       <c r="AL15" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
       <c r="AM15" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
     </row>
     <row r="16" spans="1:40">
@@ -2302,16 +2383,16 @@
         <v>924307839</v>
       </c>
       <c r="B16" t="s">
-        <v>131</v>
-      </c>
-      <c r="C16" t="s">
-        <v>69</v>
+        <v>114</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>316</v>
       </c>
       <c r="D16" s="1">
         <v>4</v>
       </c>
       <c r="E16" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="F16">
         <v>12</v>
@@ -2320,46 +2401,46 @@
         <v>2</v>
       </c>
       <c r="H16" t="s">
-        <v>56</v>
+        <v>305</v>
       </c>
       <c r="J16" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="K16" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="L16" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="O16" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="P16" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="Q16" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="AA16">
         <v>29</v>
       </c>
       <c r="AD16" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="AH16" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="AJ16" t="s">
-        <v>291</v>
+        <v>272</v>
       </c>
       <c r="AK16" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
       <c r="AL16" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
       <c r="AM16" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
     </row>
     <row r="17" spans="1:40">
@@ -2367,16 +2448,16 @@
         <v>923245192</v>
       </c>
       <c r="B17" t="s">
-        <v>140</v>
-      </c>
-      <c r="C17" t="s">
-        <v>141</v>
+        <v>123</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>318</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>290</v>
+        <v>271</v>
       </c>
       <c r="E17" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="F17">
         <v>12</v>
@@ -2385,49 +2466,49 @@
         <v>2</v>
       </c>
       <c r="H17" t="s">
-        <v>56</v>
+        <v>305</v>
       </c>
       <c r="J17" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="K17" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="L17" t="s">
-        <v>144</v>
+        <v>126</v>
       </c>
       <c r="O17" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
       <c r="P17" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
       <c r="Q17" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="AA17" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="AD17" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="AE17" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="AF17">
         <v>40241</v>
       </c>
       <c r="AJ17" t="s">
-        <v>293</v>
+        <v>274</v>
       </c>
       <c r="AK17" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
       <c r="AL17" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
       <c r="AM17" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
     </row>
     <row r="18" spans="1:40">
@@ -2435,16 +2516,16 @@
         <v>919432574</v>
       </c>
       <c r="B18" t="s">
-        <v>150</v>
-      </c>
-      <c r="C18" t="s">
-        <v>151</v>
+        <v>132</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>319</v>
       </c>
       <c r="D18" s="1">
         <v>4</v>
       </c>
       <c r="E18" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="F18">
         <v>12</v>
@@ -2453,135 +2534,150 @@
         <v>2</v>
       </c>
       <c r="H18" t="s">
-        <v>56</v>
+        <v>305</v>
       </c>
       <c r="J18" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="K18" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="L18" t="s">
-        <v>154</v>
+        <v>135</v>
       </c>
       <c r="O18" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
       <c r="P18" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="Q18" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
       <c r="AA18" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
       <c r="AB18" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
       <c r="AD18" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="AE18" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="AF18">
         <v>33901</v>
       </c>
       <c r="AJ18" t="s">
-        <v>291</v>
+        <v>272</v>
       </c>
       <c r="AK18" t="s">
-        <v>292</v>
+        <v>273</v>
       </c>
       <c r="AL18" t="s">
-        <v>292</v>
+        <v>273</v>
       </c>
       <c r="AM18" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
     </row>
     <row r="19" spans="1:40">
-      <c r="A19">
+      <c r="A19" s="4">
         <v>926287244</v>
       </c>
-      <c r="B19" t="s">
-        <v>162</v>
-      </c>
-      <c r="C19" t="s">
-        <v>82</v>
-      </c>
-      <c r="D19" s="1">
+      <c r="B19" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>314</v>
+      </c>
+      <c r="D19" s="5">
         <v>2</v>
       </c>
-      <c r="E19" t="s">
-        <v>70</v>
-      </c>
-      <c r="F19">
+      <c r="E19" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="F19" s="4">
         <v>12</v>
       </c>
-      <c r="G19" t="s">
-        <v>2</v>
-      </c>
-      <c r="H19" t="s">
-        <v>56</v>
-      </c>
-      <c r="J19" t="s">
-        <v>163</v>
-      </c>
-      <c r="K19" t="s">
-        <v>164</v>
-      </c>
-      <c r="L19" t="s">
-        <v>165</v>
-      </c>
-      <c r="O19" t="s">
-        <v>166</v>
-      </c>
-      <c r="P19" t="s">
-        <v>167</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>76</v>
-      </c>
-      <c r="R19" t="s">
-        <v>168</v>
-      </c>
-      <c r="U19" t="s">
-        <v>169</v>
-      </c>
-      <c r="V19" t="s">
-        <v>64</v>
-      </c>
-      <c r="W19">
+      <c r="G19" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="P19" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q19" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="R19" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="S19" s="4"/>
+      <c r="T19" s="4"/>
+      <c r="U19" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="V19" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="W19" s="4">
         <v>2135</v>
       </c>
-      <c r="Z19" t="s">
-        <v>170</v>
-      </c>
-      <c r="AA19" t="s">
-        <v>171</v>
-      </c>
-      <c r="AD19" t="s">
-        <v>172</v>
-      </c>
-      <c r="AE19" t="s">
-        <v>91</v>
-      </c>
-      <c r="AF19">
+      <c r="X19" s="4"/>
+      <c r="Y19" s="4"/>
+      <c r="Z19" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="AA19" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="AB19" s="4"/>
+      <c r="AC19" s="4"/>
+      <c r="AD19" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="AE19" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="AF19" s="4">
         <v>21209</v>
       </c>
-      <c r="AJ19" t="s">
-        <v>293</v>
-      </c>
-      <c r="AK19" t="s">
-        <v>292</v>
-      </c>
-      <c r="AL19" t="s">
-        <v>289</v>
-      </c>
-      <c r="AM19" t="s">
-        <v>289</v>
+      <c r="AG19" s="4"/>
+      <c r="AH19" s="4"/>
+      <c r="AI19" s="4"/>
+      <c r="AJ19" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="AK19" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="AL19" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="AM19" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="AN19" s="4" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="20" spans="1:40">
@@ -2589,55 +2685,55 @@
         <v>914664709</v>
       </c>
       <c r="B20" t="s">
-        <v>173</v>
-      </c>
-      <c r="C20" t="s">
-        <v>141</v>
+        <v>154</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>318</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="E20" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F20">
         <v>12</v>
       </c>
       <c r="G20" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="H20" t="s">
-        <v>56</v>
+        <v>305</v>
       </c>
       <c r="J20" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="K20" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="L20" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="M20" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
       <c r="N20" t="s">
-        <v>178</v>
+        <v>159</v>
       </c>
       <c r="O20" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
       <c r="P20" t="s">
-        <v>180</v>
+        <v>161</v>
       </c>
       <c r="AA20" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
       <c r="AD20" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
       <c r="AE20" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="AF20">
         <v>2420</v>
@@ -2648,16 +2744,16 @@
         <v>926789844</v>
       </c>
       <c r="B21" t="s">
-        <v>183</v>
-      </c>
-      <c r="C21" t="s">
-        <v>141</v>
+        <v>164</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>318</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="E21" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="F21">
         <v>12</v>
@@ -2666,40 +2762,40 @@
         <v>2</v>
       </c>
       <c r="H21" t="s">
-        <v>56</v>
+        <v>305</v>
       </c>
       <c r="J21" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="K21" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
       <c r="L21" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
       <c r="M21" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
       <c r="N21" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="O21" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
       <c r="P21" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="Q21" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
       <c r="AA21" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="AD21" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="AE21" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="AF21">
         <v>95014</v>
@@ -2707,48 +2803,72 @@
     </row>
     <row r="22" spans="1:40">
       <c r="B22" t="s">
-        <v>311</v>
+        <v>291</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>317</v>
       </c>
       <c r="D22" s="1">
         <v>4</v>
       </c>
+      <c r="H22" t="s">
+        <v>317</v>
+      </c>
       <c r="J22" t="s">
-        <v>312</v>
+        <v>292</v>
       </c>
       <c r="AJ22" t="s">
-        <v>292</v>
+        <v>273</v>
       </c>
       <c r="AK22" t="s">
-        <v>313</v>
+        <v>293</v>
       </c>
       <c r="AL22" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
       <c r="AM22" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
     </row>
     <row r="23" spans="1:40">
+      <c r="A23">
+        <v>915334966</v>
+      </c>
       <c r="B23" t="s">
+        <v>286</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="E23" t="s">
+        <v>40</v>
+      </c>
+      <c r="F23">
+        <v>12</v>
+      </c>
+      <c r="G23" t="s">
+        <v>41</v>
+      </c>
+      <c r="H23" t="s">
         <v>305</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>306</v>
-      </c>
       <c r="J23" t="s">
-        <v>319</v>
+        <v>299</v>
       </c>
       <c r="AJ23" t="s">
-        <v>292</v>
+        <v>273</v>
       </c>
       <c r="AK23" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
       <c r="AL23" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
       <c r="AM23" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
     </row>
     <row r="24" spans="1:40">
@@ -2756,16 +2876,16 @@
         <v>917072701</v>
       </c>
       <c r="B24" t="s">
-        <v>194</v>
-      </c>
-      <c r="C24" t="s">
-        <v>69</v>
+        <v>175</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>316</v>
       </c>
       <c r="D24" s="1">
         <v>4</v>
       </c>
       <c r="E24" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="F24">
         <v>1</v>
@@ -2774,55 +2894,55 @@
         <v>2</v>
       </c>
       <c r="H24" t="s">
-        <v>56</v>
+        <v>305</v>
       </c>
       <c r="J24" t="s">
-        <v>195</v>
+        <v>176</v>
       </c>
       <c r="K24" t="s">
-        <v>196</v>
+        <v>177</v>
       </c>
       <c r="L24" t="s">
-        <v>197</v>
+        <v>178</v>
       </c>
       <c r="M24" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
       <c r="N24" t="s">
-        <v>178</v>
+        <v>159</v>
       </c>
       <c r="O24" t="s">
-        <v>198</v>
+        <v>179</v>
       </c>
       <c r="P24" t="s">
-        <v>199</v>
+        <v>180</v>
       </c>
       <c r="Q24" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
       <c r="AA24" t="s">
-        <v>201</v>
+        <v>182</v>
       </c>
       <c r="AD24" t="s">
-        <v>202</v>
+        <v>183</v>
       </c>
       <c r="AE24" t="s">
-        <v>203</v>
+        <v>184</v>
       </c>
       <c r="AF24">
         <v>31419</v>
       </c>
       <c r="AJ24" t="s">
-        <v>293</v>
+        <v>274</v>
       </c>
       <c r="AK24" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
       <c r="AL24" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
       <c r="AM24" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
     </row>
     <row r="25" spans="1:40">
@@ -2830,16 +2950,16 @@
         <v>923156250</v>
       </c>
       <c r="B25" t="s">
-        <v>204</v>
-      </c>
-      <c r="C25" t="s">
-        <v>69</v>
+        <v>185</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>316</v>
       </c>
       <c r="D25" s="1">
         <v>3</v>
       </c>
       <c r="E25" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="F25">
         <v>12</v>
@@ -2848,66 +2968,66 @@
         <v>2</v>
       </c>
       <c r="H25" t="s">
-        <v>56</v>
+        <v>305</v>
       </c>
       <c r="J25" t="s">
-        <v>205</v>
+        <v>186</v>
       </c>
       <c r="K25" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="L25" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="O25" t="s">
-        <v>206</v>
+        <v>187</v>
       </c>
       <c r="P25" t="s">
-        <v>207</v>
+        <v>188</v>
       </c>
       <c r="Q25" t="s">
-        <v>208</v>
+        <v>189</v>
       </c>
       <c r="AA25" t="s">
-        <v>209</v>
+        <v>190</v>
       </c>
       <c r="AD25" t="s">
-        <v>210</v>
+        <v>191</v>
       </c>
       <c r="AE25" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="AF25">
         <v>90503</v>
       </c>
       <c r="AJ25" t="s">
-        <v>293</v>
+        <v>274</v>
       </c>
       <c r="AK25" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
       <c r="AL25" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
       <c r="AM25" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
     </row>
-    <row r="26" spans="1:40">
+    <row r="26" spans="1:40" s="4" customFormat="1">
       <c r="A26">
         <v>923716852</v>
       </c>
       <c r="B26" t="s">
-        <v>211</v>
-      </c>
-      <c r="C26" t="s">
-        <v>69</v>
+        <v>192</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>316</v>
       </c>
       <c r="D26" s="1">
         <v>4</v>
       </c>
       <c r="E26" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="F26">
         <v>12</v>
@@ -2916,690 +3036,800 @@
         <v>2</v>
       </c>
       <c r="H26" t="s">
-        <v>56</v>
-      </c>
+        <v>305</v>
+      </c>
+      <c r="I26"/>
       <c r="J26" t="s">
-        <v>212</v>
+        <v>193</v>
       </c>
       <c r="K26" t="s">
-        <v>213</v>
+        <v>194</v>
       </c>
       <c r="L26" t="s">
-        <v>214</v>
+        <v>195</v>
       </c>
       <c r="M26" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="N26" t="s">
-        <v>216</v>
+        <v>197</v>
       </c>
       <c r="O26" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="P26" t="s">
-        <v>218</v>
+        <v>199</v>
       </c>
       <c r="Q26" t="s">
-        <v>219</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="R26"/>
+      <c r="S26"/>
+      <c r="T26"/>
+      <c r="U26"/>
+      <c r="V26"/>
+      <c r="W26"/>
+      <c r="X26"/>
+      <c r="Y26"/>
+      <c r="Z26"/>
       <c r="AA26" t="s">
-        <v>220</v>
-      </c>
+        <v>201</v>
+      </c>
+      <c r="AB26"/>
+      <c r="AC26"/>
       <c r="AD26" t="s">
-        <v>221</v>
+        <v>202</v>
       </c>
       <c r="AE26" t="s">
-        <v>222</v>
+        <v>203</v>
       </c>
       <c r="AF26">
         <v>98383</v>
       </c>
+      <c r="AG26"/>
+      <c r="AH26"/>
+      <c r="AI26"/>
       <c r="AJ26" t="s">
-        <v>292</v>
+        <v>273</v>
       </c>
       <c r="AK26" t="s">
-        <v>292</v>
+        <v>273</v>
       </c>
       <c r="AL26" t="s">
-        <v>292</v>
+        <v>273</v>
       </c>
       <c r="AM26" t="s">
-        <v>289</v>
-      </c>
+        <v>270</v>
+      </c>
+      <c r="AN26"/>
     </row>
     <row r="27" spans="1:40">
-      <c r="A27">
+      <c r="A27" s="4">
         <v>911661305</v>
       </c>
-      <c r="B27" t="s">
-        <v>223</v>
-      </c>
-      <c r="C27" t="s">
-        <v>82</v>
-      </c>
-      <c r="D27" s="1">
+      <c r="B27" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>314</v>
+      </c>
+      <c r="D27" s="5">
         <v>4</v>
       </c>
-      <c r="E27" t="s">
-        <v>70</v>
-      </c>
-      <c r="F27">
+      <c r="E27" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="F27" s="4">
         <v>12</v>
       </c>
-      <c r="G27" t="s">
-        <v>2</v>
-      </c>
-      <c r="H27" t="s">
-        <v>56</v>
-      </c>
-      <c r="J27" t="s">
-        <v>224</v>
-      </c>
-      <c r="K27" t="s">
-        <v>225</v>
-      </c>
-      <c r="L27" t="s">
-        <v>226</v>
-      </c>
-      <c r="O27" t="s">
-        <v>227</v>
-      </c>
-      <c r="P27" t="s">
-        <v>228</v>
-      </c>
-      <c r="R27" t="s">
-        <v>229</v>
-      </c>
-      <c r="U27" t="s">
-        <v>114</v>
-      </c>
-      <c r="V27" t="s">
-        <v>64</v>
-      </c>
-      <c r="W27">
+      <c r="G27" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="L27" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="P27" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="Q27" s="4"/>
+      <c r="R27" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="S27" s="4"/>
+      <c r="T27" s="4"/>
+      <c r="U27" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="V27" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="W27" s="4">
         <v>2215</v>
       </c>
-      <c r="Z27" t="s">
-        <v>230</v>
-      </c>
-      <c r="AA27" t="s">
-        <v>231</v>
-      </c>
-      <c r="AD27" t="s">
-        <v>232</v>
-      </c>
-      <c r="AE27" t="s">
-        <v>67</v>
-      </c>
-      <c r="AF27">
+      <c r="X27" s="4"/>
+      <c r="Y27" s="4"/>
+      <c r="Z27" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="AA27" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="AB27" s="4"/>
+      <c r="AC27" s="4"/>
+      <c r="AD27" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="AE27" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF27" s="4">
         <v>22101</v>
+      </c>
+      <c r="AG27" s="4"/>
+      <c r="AH27" s="4"/>
+      <c r="AI27" s="4"/>
+      <c r="AJ27" s="4"/>
+      <c r="AK27" s="4"/>
+      <c r="AL27" s="4"/>
+      <c r="AM27" s="4"/>
+      <c r="AN27" s="4" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="28" spans="1:40">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4" t="s">
-        <v>298</v>
-      </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="5" t="s">
-        <v>300</v>
-      </c>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4" t="s">
-        <v>299</v>
-      </c>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
-      <c r="P28" s="4"/>
-      <c r="Q28" s="4"/>
-      <c r="R28" s="4"/>
-      <c r="S28" s="4"/>
-      <c r="T28" s="4"/>
-      <c r="U28" s="4"/>
-      <c r="V28" s="4"/>
-      <c r="W28" s="4"/>
-      <c r="X28" s="4"/>
-      <c r="Y28" s="4"/>
-      <c r="Z28" s="4"/>
-      <c r="AA28" s="4"/>
-      <c r="AB28" s="4"/>
-      <c r="AC28" s="4"/>
-      <c r="AD28" s="4"/>
-      <c r="AE28" s="4"/>
-      <c r="AF28" s="4"/>
-      <c r="AG28" s="4"/>
-      <c r="AH28" s="4"/>
-      <c r="AI28" s="4"/>
-      <c r="AJ28" s="4" t="s">
-        <v>293</v>
-      </c>
-      <c r="AK28" s="4" t="s">
-        <v>289</v>
-      </c>
-      <c r="AL28" s="4" t="s">
-        <v>289</v>
-      </c>
-      <c r="AM28" s="4" t="s">
-        <v>289</v>
-      </c>
-      <c r="AN28" s="4" t="s">
-        <v>323</v>
+      <c r="A28">
+        <v>910716246</v>
+      </c>
+      <c r="B28" t="s">
+        <v>310</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="D28">
+        <v>3</v>
+      </c>
+      <c r="E28" t="s">
+        <v>54</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="H28" t="s">
+        <v>305</v>
+      </c>
+      <c r="J28" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="29" spans="1:40">
-      <c r="A29">
-        <v>925196770</v>
-      </c>
-      <c r="B29" t="s">
-        <v>233</v>
-      </c>
-      <c r="C29" t="s">
-        <v>82</v>
-      </c>
-      <c r="D29" s="1">
-        <v>2</v>
-      </c>
-      <c r="E29" t="s">
-        <v>70</v>
-      </c>
-      <c r="F29">
-        <v>12</v>
-      </c>
-      <c r="G29" t="s">
-        <v>2</v>
-      </c>
-      <c r="H29" t="s">
-        <v>56</v>
-      </c>
-      <c r="J29" t="s">
-        <v>234</v>
-      </c>
-      <c r="K29" t="s">
-        <v>235</v>
-      </c>
-      <c r="L29" t="s">
-        <v>236</v>
-      </c>
-      <c r="M29" t="s">
-        <v>123</v>
-      </c>
-      <c r="N29" t="s">
-        <v>124</v>
-      </c>
-      <c r="O29" t="s">
-        <v>237</v>
-      </c>
-      <c r="P29" t="s">
-        <v>238</v>
-      </c>
-      <c r="AA29" t="s">
-        <v>239</v>
-      </c>
-      <c r="AD29" t="s">
-        <v>240</v>
-      </c>
-      <c r="AE29" t="s">
-        <v>118</v>
-      </c>
-      <c r="AF29">
-        <v>95138</v>
-      </c>
-      <c r="AJ29" t="s">
-        <v>289</v>
-      </c>
-      <c r="AK29" t="s">
-        <v>289</v>
-      </c>
-      <c r="AL29" t="s">
-        <v>289</v>
-      </c>
-      <c r="AM29" t="s">
-        <v>289</v>
+      <c r="A29" s="4"/>
+      <c r="B29" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4"/>
+      <c r="R29" s="4"/>
+      <c r="S29" s="4"/>
+      <c r="T29" s="4"/>
+      <c r="U29" s="4"/>
+      <c r="V29" s="4"/>
+      <c r="W29" s="4"/>
+      <c r="X29" s="4"/>
+      <c r="Y29" s="4"/>
+      <c r="Z29" s="4"/>
+      <c r="AA29" s="4"/>
+      <c r="AB29" s="4"/>
+      <c r="AC29" s="4"/>
+      <c r="AD29" s="4"/>
+      <c r="AE29" s="4"/>
+      <c r="AF29" s="4"/>
+      <c r="AG29" s="4"/>
+      <c r="AH29" s="4"/>
+      <c r="AI29" s="4"/>
+      <c r="AJ29" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="AK29" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="AL29" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="AM29" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="AN29" s="4" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="30" spans="1:40">
+      <c r="A30">
+        <v>925196770</v>
+      </c>
       <c r="B30" t="s">
-        <v>301</v>
+        <v>214</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>314</v>
       </c>
       <c r="D30" s="1">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="E30" t="s">
+        <v>54</v>
+      </c>
+      <c r="F30">
+        <v>12</v>
+      </c>
+      <c r="G30" t="s">
+        <v>2</v>
+      </c>
+      <c r="H30" t="s">
+        <v>305</v>
       </c>
       <c r="J30" t="s">
-        <v>321</v>
+        <v>215</v>
+      </c>
+      <c r="K30" t="s">
+        <v>216</v>
+      </c>
+      <c r="L30" t="s">
+        <v>217</v>
+      </c>
+      <c r="M30" t="s">
+        <v>106</v>
+      </c>
+      <c r="N30" t="s">
+        <v>107</v>
+      </c>
+      <c r="O30" t="s">
+        <v>218</v>
+      </c>
+      <c r="P30" t="s">
+        <v>219</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>220</v>
+      </c>
+      <c r="AD30" t="s">
+        <v>221</v>
+      </c>
+      <c r="AE30" t="s">
+        <v>101</v>
+      </c>
+      <c r="AF30">
+        <v>95138</v>
       </c>
       <c r="AJ30" t="s">
-        <v>291</v>
+        <v>270</v>
       </c>
       <c r="AK30" t="s">
-        <v>292</v>
+        <v>270</v>
       </c>
       <c r="AL30" t="s">
-        <v>292</v>
+        <v>270</v>
       </c>
       <c r="AM30" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
     </row>
     <row r="31" spans="1:40">
-      <c r="A31">
-        <v>925337783</v>
-      </c>
       <c r="B31" t="s">
-        <v>241</v>
-      </c>
-      <c r="C31" t="s">
-        <v>141</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="E31" t="s">
-        <v>70</v>
-      </c>
-      <c r="F31">
-        <v>12</v>
-      </c>
-      <c r="G31" t="s">
-        <v>2</v>
+        <v>282</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="D31" s="1">
+        <v>4</v>
       </c>
       <c r="H31" t="s">
-        <v>56</v>
+        <v>317</v>
       </c>
       <c r="J31" t="s">
-        <v>242</v>
-      </c>
-      <c r="K31" t="s">
-        <v>143</v>
-      </c>
-      <c r="L31" t="s">
-        <v>144</v>
-      </c>
-      <c r="M31" t="s">
-        <v>187</v>
-      </c>
-      <c r="N31" t="s">
-        <v>188</v>
-      </c>
-      <c r="O31" t="s">
-        <v>243</v>
-      </c>
-      <c r="P31" t="s">
-        <v>244</v>
-      </c>
-      <c r="Q31" t="s">
-        <v>245</v>
-      </c>
-      <c r="AA31" t="s">
-        <v>246</v>
-      </c>
-      <c r="AD31" t="s">
-        <v>240</v>
-      </c>
-      <c r="AE31" t="s">
-        <v>118</v>
-      </c>
-      <c r="AF31">
-        <v>95126</v>
+        <v>301</v>
       </c>
       <c r="AJ31" t="s">
-        <v>289</v>
+        <v>272</v>
       </c>
       <c r="AK31" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
       <c r="AL31" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
       <c r="AM31" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
     </row>
     <row r="32" spans="1:40">
+      <c r="A32">
+        <v>925337783</v>
+      </c>
       <c r="B32" t="s">
-        <v>314</v>
-      </c>
-      <c r="D32" s="1">
-        <v>4</v>
+        <v>222</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="E32" t="s">
+        <v>54</v>
+      </c>
+      <c r="F32">
+        <v>12</v>
+      </c>
+      <c r="G32" t="s">
+        <v>2</v>
+      </c>
+      <c r="H32" t="s">
+        <v>305</v>
       </c>
       <c r="J32" t="s">
-        <v>315</v>
+        <v>223</v>
+      </c>
+      <c r="K32" t="s">
+        <v>125</v>
+      </c>
+      <c r="L32" t="s">
+        <v>126</v>
+      </c>
+      <c r="M32" t="s">
+        <v>168</v>
+      </c>
+      <c r="N32" t="s">
+        <v>169</v>
+      </c>
+      <c r="O32" t="s">
+        <v>224</v>
+      </c>
+      <c r="P32" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>226</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>227</v>
+      </c>
+      <c r="AD32" t="s">
+        <v>221</v>
+      </c>
+      <c r="AE32" t="s">
+        <v>101</v>
+      </c>
+      <c r="AF32">
+        <v>95126</v>
       </c>
       <c r="AJ32" t="s">
-        <v>313</v>
+        <v>270</v>
       </c>
       <c r="AK32" t="s">
-        <v>313</v>
+        <v>270</v>
       </c>
       <c r="AL32" t="s">
-        <v>292</v>
+        <v>270</v>
       </c>
       <c r="AM32" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
     </row>
     <row r="33" spans="1:39">
-      <c r="A33">
-        <v>920690945</v>
-      </c>
       <c r="B33" t="s">
-        <v>247</v>
-      </c>
-      <c r="C33" t="s">
-        <v>82</v>
+        <v>294</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>317</v>
       </c>
       <c r="D33" s="1">
-        <v>3</v>
-      </c>
-      <c r="E33" t="s">
-        <v>70</v>
-      </c>
-      <c r="F33">
-        <v>12</v>
-      </c>
-      <c r="G33" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H33" t="s">
-        <v>56</v>
+        <v>317</v>
       </c>
       <c r="J33" t="s">
-        <v>248</v>
-      </c>
-      <c r="K33" t="s">
-        <v>249</v>
-      </c>
-      <c r="L33" t="s">
-        <v>250</v>
-      </c>
-      <c r="M33" t="s">
-        <v>251</v>
-      </c>
-      <c r="N33" t="s">
-        <v>252</v>
-      </c>
-      <c r="O33" t="s">
-        <v>253</v>
-      </c>
-      <c r="P33" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q33" t="s">
-        <v>254</v>
-      </c>
-      <c r="Z33" t="s">
-        <v>255</v>
-      </c>
-      <c r="AA33" t="s">
-        <v>256</v>
-      </c>
-      <c r="AD33" t="s">
-        <v>257</v>
-      </c>
-      <c r="AE33" t="s">
-        <v>91</v>
-      </c>
-      <c r="AF33">
-        <v>21048</v>
+        <v>295</v>
       </c>
       <c r="AJ33" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="AK33" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="AL33" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
       <c r="AM33" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
     </row>
     <row r="34" spans="1:39">
       <c r="A34">
-        <v>929035252</v>
+        <v>912666162</v>
       </c>
       <c r="B34" t="s">
-        <v>258</v>
-      </c>
-      <c r="C34" t="s">
-        <v>141</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>53</v>
+        <v>312</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="D34" t="s">
+        <v>39</v>
       </c>
       <c r="E34" t="s">
         <v>54</v>
       </c>
       <c r="F34">
-        <v>1</v>
-      </c>
-      <c r="G34" t="s">
-        <v>55</v>
+        <v>12</v>
       </c>
       <c r="H34" t="s">
-        <v>56</v>
+        <v>305</v>
       </c>
       <c r="J34" t="s">
-        <v>259</v>
-      </c>
-      <c r="K34" t="s">
-        <v>260</v>
-      </c>
-      <c r="L34" t="s">
-        <v>261</v>
-      </c>
-      <c r="O34" t="s">
-        <v>262</v>
-      </c>
-      <c r="P34" t="s">
-        <v>263</v>
-      </c>
-      <c r="Q34" t="s">
-        <v>76</v>
-      </c>
-      <c r="R34" t="s">
-        <v>264</v>
-      </c>
-      <c r="U34" t="s">
-        <v>63</v>
-      </c>
-      <c r="V34" t="s">
-        <v>64</v>
-      </c>
-      <c r="W34">
-        <v>2139</v>
-      </c>
-      <c r="Z34" t="s">
-        <v>265</v>
-      </c>
-      <c r="AA34" t="s">
-        <v>266</v>
-      </c>
-      <c r="AD34" t="s">
-        <v>267</v>
-      </c>
-      <c r="AE34" t="s">
-        <v>118</v>
-      </c>
-      <c r="AF34">
-        <v>91770</v>
+        <v>313</v>
       </c>
     </row>
     <row r="35" spans="1:39">
+      <c r="A35">
+        <v>920690945</v>
+      </c>
       <c r="B35" t="s">
-        <v>316</v>
+        <v>228</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>314</v>
       </c>
       <c r="D35" s="1">
         <v>3</v>
       </c>
+      <c r="E35" t="s">
+        <v>54</v>
+      </c>
+      <c r="F35">
+        <v>12</v>
+      </c>
+      <c r="G35" t="s">
+        <v>2</v>
+      </c>
+      <c r="H35" t="s">
+        <v>305</v>
+      </c>
       <c r="J35" t="s">
-        <v>318</v>
+        <v>229</v>
+      </c>
+      <c r="K35" t="s">
+        <v>230</v>
+      </c>
+      <c r="L35" t="s">
+        <v>231</v>
+      </c>
+      <c r="M35" t="s">
+        <v>232</v>
+      </c>
+      <c r="N35" t="s">
+        <v>233</v>
+      </c>
+      <c r="O35" t="s">
+        <v>234</v>
+      </c>
+      <c r="P35" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>235</v>
+      </c>
+      <c r="Z35" t="s">
+        <v>236</v>
+      </c>
+      <c r="AA35" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD35" t="s">
+        <v>238</v>
+      </c>
+      <c r="AE35" t="s">
+        <v>74</v>
+      </c>
+      <c r="AF35">
+        <v>21048</v>
       </c>
       <c r="AJ35" t="s">
-        <v>291</v>
+        <v>270</v>
       </c>
       <c r="AK35" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
       <c r="AL35" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
       <c r="AM35" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
     </row>
     <row r="36" spans="1:39">
       <c r="A36">
-        <v>923932731</v>
+        <v>929035252</v>
       </c>
       <c r="B36" t="s">
-        <v>268</v>
-      </c>
-      <c r="C36" t="s">
-        <v>69</v>
-      </c>
-      <c r="D36" s="1">
-        <v>4</v>
+        <v>239</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="E36" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="F36">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="G36" t="s">
-        <v>2</v>
+        <v>41</v>
       </c>
       <c r="H36" t="s">
-        <v>56</v>
+        <v>305</v>
       </c>
       <c r="J36" t="s">
-        <v>269</v>
+        <v>240</v>
       </c>
       <c r="K36" t="s">
-        <v>225</v>
+        <v>241</v>
       </c>
       <c r="L36" t="s">
-        <v>226</v>
-      </c>
-      <c r="M36" t="s">
-        <v>270</v>
-      </c>
-      <c r="N36" t="s">
-        <v>271</v>
+        <v>242</v>
       </c>
       <c r="O36" t="s">
-        <v>272</v>
+        <v>243</v>
       </c>
       <c r="P36" t="s">
-        <v>273</v>
+        <v>244</v>
       </c>
       <c r="Q36" t="s">
-        <v>88</v>
+        <v>60</v>
+      </c>
+      <c r="R36" t="s">
+        <v>245</v>
+      </c>
+      <c r="U36" t="s">
+        <v>48</v>
+      </c>
+      <c r="V36" t="s">
+        <v>49</v>
+      </c>
+      <c r="W36">
+        <v>2139</v>
+      </c>
+      <c r="Z36" t="s">
+        <v>246</v>
       </c>
       <c r="AA36" t="s">
-        <v>274</v>
+        <v>247</v>
       </c>
       <c r="AD36" t="s">
-        <v>275</v>
+        <v>248</v>
       </c>
       <c r="AE36" t="s">
-        <v>64</v>
+        <v>101</v>
       </c>
       <c r="AF36">
-        <v>2482</v>
-      </c>
-      <c r="AJ36" t="s">
-        <v>291</v>
-      </c>
-      <c r="AK36" t="s">
-        <v>289</v>
-      </c>
-      <c r="AL36" t="s">
-        <v>289</v>
-      </c>
-      <c r="AM36" t="s">
-        <v>289</v>
+        <v>91770</v>
       </c>
     </row>
     <row r="37" spans="1:39">
-      <c r="A37">
+      <c r="B37" t="s">
+        <v>296</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="D37" s="1">
+        <v>3</v>
+      </c>
+      <c r="H37" t="s">
+        <v>317</v>
+      </c>
+      <c r="J37" t="s">
+        <v>298</v>
+      </c>
+      <c r="AJ37" t="s">
+        <v>272</v>
+      </c>
+      <c r="AK37" t="s">
+        <v>270</v>
+      </c>
+      <c r="AL37" t="s">
+        <v>270</v>
+      </c>
+      <c r="AM37" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="38" spans="1:39">
+      <c r="A38">
+        <v>923932731</v>
+      </c>
+      <c r="B38" t="s">
+        <v>249</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="D38" s="1">
+        <v>4</v>
+      </c>
+      <c r="E38" t="s">
+        <v>54</v>
+      </c>
+      <c r="F38">
+        <v>12</v>
+      </c>
+      <c r="G38" t="s">
+        <v>2</v>
+      </c>
+      <c r="H38" t="s">
+        <v>305</v>
+      </c>
+      <c r="J38" t="s">
+        <v>250</v>
+      </c>
+      <c r="K38" t="s">
+        <v>206</v>
+      </c>
+      <c r="L38" t="s">
+        <v>207</v>
+      </c>
+      <c r="M38" t="s">
+        <v>251</v>
+      </c>
+      <c r="N38" t="s">
+        <v>252</v>
+      </c>
+      <c r="O38" t="s">
+        <v>253</v>
+      </c>
+      <c r="P38" t="s">
+        <v>254</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA38" t="s">
+        <v>255</v>
+      </c>
+      <c r="AD38" t="s">
+        <v>256</v>
+      </c>
+      <c r="AE38" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF38">
+        <v>2482</v>
+      </c>
+      <c r="AJ38" t="s">
+        <v>272</v>
+      </c>
+      <c r="AK38" t="s">
+        <v>270</v>
+      </c>
+      <c r="AL38" t="s">
+        <v>270</v>
+      </c>
+      <c r="AM38" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="39" spans="1:39">
+      <c r="A39">
         <v>929406802</v>
       </c>
-      <c r="B37" t="s">
-        <v>276</v>
-      </c>
-      <c r="C37" t="s">
-        <v>141</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E37" t="s">
-        <v>70</v>
-      </c>
-      <c r="F37">
+      <c r="B39" t="s">
+        <v>257</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E39" t="s">
+        <v>54</v>
+      </c>
+      <c r="F39">
         <v>12</v>
       </c>
-      <c r="G37" t="s">
+      <c r="G39" t="s">
         <v>2</v>
       </c>
-      <c r="H37" t="s">
-        <v>56</v>
-      </c>
-      <c r="J37" t="s">
-        <v>277</v>
-      </c>
-      <c r="K37" t="s">
-        <v>278</v>
-      </c>
-      <c r="L37" t="s">
-        <v>279</v>
-      </c>
-      <c r="O37" t="s">
-        <v>280</v>
-      </c>
-      <c r="P37" t="s">
-        <v>281</v>
-      </c>
-      <c r="R37" t="s">
-        <v>282</v>
-      </c>
-      <c r="U37" t="s">
-        <v>63</v>
-      </c>
-      <c r="V37" t="s">
-        <v>64</v>
-      </c>
-      <c r="W37">
+      <c r="H39" t="s">
+        <v>305</v>
+      </c>
+      <c r="J39" t="s">
+        <v>258</v>
+      </c>
+      <c r="K39" t="s">
+        <v>259</v>
+      </c>
+      <c r="L39" t="s">
+        <v>260</v>
+      </c>
+      <c r="O39" t="s">
+        <v>261</v>
+      </c>
+      <c r="P39" t="s">
+        <v>262</v>
+      </c>
+      <c r="R39" t="s">
+        <v>263</v>
+      </c>
+      <c r="U39" t="s">
+        <v>48</v>
+      </c>
+      <c r="V39" t="s">
+        <v>49</v>
+      </c>
+      <c r="W39">
         <v>2139</v>
       </c>
-      <c r="Z37" t="s">
-        <v>283</v>
-      </c>
-      <c r="AA37" t="s">
-        <v>284</v>
-      </c>
-      <c r="AB37" t="s">
-        <v>285</v>
-      </c>
-      <c r="AD37" t="s">
-        <v>286</v>
-      </c>
-      <c r="AH37" t="s">
-        <v>287</v>
+      <c r="Z39" t="s">
+        <v>264</v>
+      </c>
+      <c r="AA39" t="s">
+        <v>265</v>
+      </c>
+      <c r="AB39" t="s">
+        <v>266</v>
+      </c>
+      <c r="AD39" t="s">
+        <v>267</v>
+      </c>
+      <c r="AH39" t="s">
+        <v>268</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A6:AM37">
-    <sortCondition ref="B6:B37"/>
+  <sortState ref="A5:AN41">
+    <sortCondition ref="B5:B41"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>